<commit_message>
working on db models (3 tables planned)
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640496A8-2DC0-44B3-BD4E-6E9D7E175989}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E90441-C7E6-42C4-9C0A-A2588F4F6060}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>stories</t>
   </si>
   <si>
-    <t>creatures</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>sqlite only good for dev</t>
+  </si>
+  <si>
+    <t>being</t>
   </si>
 </sst>
 </file>
@@ -785,7 +785,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="48"/>
       <c r="K1" s="30"/>
@@ -820,22 +820,22 @@
         <v>2</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="42" t="s">
         <v>44</v>
-      </c>
-      <c r="S1" s="42" t="s">
-        <v>45</v>
       </c>
       <c r="T1" s="42"/>
       <c r="U1" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V1" s="43"/>
     </row>
@@ -852,16 +852,16 @@
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>3</v>
@@ -869,7 +869,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="8"/>
       <c r="U2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -886,14 +886,14 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="O3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="8"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="7"/>
@@ -927,7 +927,7 @@
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
@@ -937,14 +937,14 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -979,7 +979,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1076,7 +1076,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1151,24 +1151,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="35" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
       <c r="L16" s="33"/>
       <c r="M16" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="20"/>
@@ -1178,30 +1178,30 @@
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="7"/>
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="7"/>
       <c r="L17" s="36"/>
       <c r="M17" s="21"/>
       <c r="N17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="8"/>
@@ -1209,29 +1209,29 @@
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4"/>
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="37"/>
       <c r="M18" s="27"/>
       <c r="N18" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O18" s="29"/>
       <c r="P18" s="7"/>
@@ -1240,7 +1240,7 @@
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8"/>
@@ -1248,17 +1248,17 @@
       <c r="F19" s="2"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
       <c r="L19" s="39"/>
       <c r="M19" s="22"/>
       <c r="N19" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O19" s="24"/>
       <c r="P19" s="7"/>
@@ -1275,7 +1275,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="6"/>
       <c r="H20" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="8"/>
@@ -1290,7 +1290,7 @@
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
@@ -1321,7 +1321,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
@@ -1414,7 +1414,7 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="8"/>
@@ -1422,7 +1422,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
@@ -1430,7 +1430,7 @@
       <c r="L27" s="39"/>
       <c r="M27" s="39"/>
       <c r="N27" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O27" s="40"/>
       <c r="P27" s="40"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1465,7 +1465,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="2"/>
       <c r="G29" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>

</xml_diff>

<commit_message>
trying to set up story and being tables with relationships...
https://docs.sqlalchemy.org/en/latest/orm/basic_relationships.html
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E90441-C7E6-42C4-9C0A-A2588F4F6060}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B50856-CA90-464B-B126-54462A7D7977}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>MAIN</t>
   </si>
@@ -90,9 +90,6 @@
     <t>primary</t>
   </si>
   <si>
-    <t>optional</t>
-  </si>
-  <si>
     <t>CRUD</t>
   </si>
   <si>
@@ -175,13 +172,28 @@
   </si>
   <si>
     <t>being</t>
+  </si>
+  <si>
+    <t>example: zeus is in many stories, no point in linking him to one in particular</t>
+  </si>
+  <si>
+    <t>indexes</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +235,15 @@
       <b/>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -468,6 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0752C00-C314-4AC1-BFCC-C3E780D9EA50}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="N29" sqref="N29:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +833,7 @@
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="48"/>
       <c r="K1" s="30"/>
@@ -820,22 +842,22 @@
         <v>2</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="42" t="s">
         <v>43</v>
-      </c>
-      <c r="S1" s="42" t="s">
-        <v>44</v>
       </c>
       <c r="T1" s="42"/>
       <c r="U1" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V1" s="43"/>
     </row>
@@ -861,7 +883,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>3</v>
@@ -869,7 +891,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="8"/>
       <c r="U2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -886,14 +908,14 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="O3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="8"/>
@@ -911,7 +933,7 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="7"/>
@@ -927,7 +949,7 @@
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
@@ -937,14 +959,14 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
@@ -971,7 +993,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -979,7 +1001,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1076,7 +1098,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1151,24 +1173,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
       <c r="L16" s="33"/>
       <c r="M16" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="20"/>
@@ -1198,10 +1220,10 @@
       <c r="L17" s="36"/>
       <c r="M17" s="21"/>
       <c r="N17" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="8"/>
@@ -1218,20 +1240,18 @@
       <c r="E18" s="4"/>
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="J18" s="5"/>
       <c r="K18" s="7"/>
       <c r="L18" s="37"/>
       <c r="M18" s="27"/>
       <c r="N18" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O18" s="29"/>
       <c r="P18" s="7"/>
@@ -1240,7 +1260,7 @@
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8"/>
@@ -1258,7 +1278,7 @@
       <c r="L19" s="39"/>
       <c r="M19" s="22"/>
       <c r="N19" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O19" s="24"/>
       <c r="P19" s="7"/>
@@ -1275,7 +1295,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="6"/>
       <c r="H20" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="8"/>
@@ -1290,7 +1310,7 @@
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
@@ -1321,14 +1341,18 @@
       <c r="F22" s="2"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
       <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
+      <c r="M22" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>51</v>
+      </c>
       <c r="O22" s="33"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="8"/>
@@ -1349,7 +1373,9 @@
       <c r="K23" s="7"/>
       <c r="L23" s="33"/>
       <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
+      <c r="N23" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="O23" s="33"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="8"/>
@@ -1368,7 +1394,9 @@
       <c r="K24" s="7"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
+      <c r="N24" s="33" t="s">
+        <v>52</v>
+      </c>
       <c r="O24" s="33"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="8"/>
@@ -1387,7 +1415,9 @@
       <c r="K25" s="7"/>
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
+      <c r="N25" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="O25" s="33"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="8"/>
@@ -1406,7 +1436,9 @@
       <c r="K26" s="7"/>
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
+      <c r="N26" s="33" t="s">
+        <v>53</v>
+      </c>
       <c r="O26" s="33"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="8"/>
@@ -1414,7 +1446,7 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="8"/>
@@ -1422,18 +1454,13 @@
       <c r="F27" s="2"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
       <c r="K27" s="7"/>
       <c r="L27" s="39"/>
       <c r="M27" s="39"/>
-      <c r="N27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
       <c r="Q27" s="8"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1450,14 +1477,11 @@
       <c r="K28" s="7"/>
       <c r="L28" s="33"/>
       <c r="M28" s="33"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
       <c r="Q28" s="8"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1465,7 +1489,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="2"/>
       <c r="G29" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -1473,9 +1497,11 @@
       <c r="K29" s="7"/>
       <c r="L29" s="33"/>
       <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="7"/>
+      <c r="N29" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1492,9 +1518,9 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
       <c r="Q30" s="8"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1516,6 +1542,11 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="11"/>
     </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
working on users views.py and database
https://flask-login.readthedocs.io/en/latest/ /// user_loader callback typo
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B50856-CA90-464B-B126-54462A7D7977}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74592B02-1DE4-4FE4-BCF8-5B9D1D2DA8B4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -804,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0752C00-C314-4AC1-BFCC-C3E780D9EA50}">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29:P30"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1529,9 @@
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
@@ -1542,11 +1544,6 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="11"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
added img + working on ui/ux of views
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8A57B-A574-4169-A818-C606FBEB4696}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D85817-2D62-4AD0-B70F-C0A2555F2B0E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>MAIN</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>OTHERS</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -1634,10 +1637,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C059251-7E5B-47F6-9A8F-E7A0BC421FB2}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,6 +1703,9 @@
       <c r="A3" t="s">
         <v>55</v>
       </c>
+      <c r="G3" s="55" t="s">
+        <v>62</v>
+      </c>
       <c r="M3" s="55" t="s">
         <v>60</v>
       </c>
@@ -1704,6 +1713,9 @@
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
+      </c>
+      <c r="M4" s="55" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolving update screen validation bug by allowing only username change
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D85817-2D62-4AD0-B70F-C0A2555F2B0E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B102B9-B3D9-4054-BA31-16F7D1F506B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>MAIN</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>update</t>
+  </si>
+  <si>
+    <t>update validation</t>
+  </si>
+  <si>
+    <t>add pagination for entries</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -575,6 +581,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1643,7 +1650,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,24 +1705,25 @@
       <c r="M2" s="55" t="s">
         <v>59</v>
       </c>
+      <c r="T2" s="55" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="55" t="s">
-        <v>62</v>
-      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
       <c r="M3" s="55" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="60" t="s">
         <v>58</v>
-      </c>
-      <c r="M4" s="55" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update users views and create html pages associated + login.html url
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B102B9-B3D9-4054-BA31-16F7D1F506B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D6FB64-6F0A-4AD8-A28E-025B6D16995A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>MAIN</t>
   </si>
@@ -214,13 +214,13 @@
     <t>OTHERS</t>
   </si>
   <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>update validation</t>
-  </si>
-  <si>
     <t>add pagination for entries</t>
+  </si>
+  <si>
+    <t>password retrieval or reset</t>
+  </si>
+  <si>
+    <t>contact form</t>
   </si>
 </sst>
 </file>
@@ -1647,10 +1647,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1706,7 @@
         <v>59</v>
       </c>
       <c r="T2" s="55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1720,10 +1720,18 @@
       <c r="M3" s="55" t="s">
         <v>60</v>
       </c>
+      <c r="T3" s="55" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparing db change from sqlite to postgresql
</commit_message>
<xml_diff>
--- a/amphora/database_model_planning.xlsx
+++ b/amphora/database_model_planning.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_DataCentric\CI_DataCentric\amphora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D6FB64-6F0A-4AD8-A28E-025B6D16995A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F444B7F-0D34-4A5C-BDBB-E1F1140A840D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3AD21F7F-35A0-43FA-A285-D59E266D033A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="TO DO LIST" sheetId="2" r:id="rId2"/>
+    <sheet name="Database structure" sheetId="3" r:id="rId1"/>
+    <sheet name="Plan" sheetId="1" r:id="rId2"/>
+    <sheet name="TO DO LIST" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>MAIN</t>
   </si>
@@ -67,9 +68,6 @@
     <t>Repository (collection of entries)</t>
   </si>
   <si>
-    <t>country of origin</t>
-  </si>
-  <si>
     <t>variations</t>
   </si>
   <si>
@@ -148,9 +146,6 @@
     <t>body of text</t>
   </si>
   <si>
-    <t>table of countries; potentially search option</t>
-  </si>
-  <si>
     <t>cultural affiliation, theme</t>
   </si>
   <si>
@@ -221,13 +216,91 @@
   </si>
   <si>
     <t>contact form</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Being</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>psw_hash</t>
+  </si>
+  <si>
+    <t>beings</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>foreignkey</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>repr</t>
+  </si>
+  <si>
+    <t>set_password</t>
+  </si>
+  <si>
+    <t>password_check</t>
+  </si>
+  <si>
+    <t>get_psw_token</t>
+  </si>
+  <si>
+    <t>verify_psw_token</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>being_id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>meaning and values</t>
+  </si>
+  <si>
+    <t>comments??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +359,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -520,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -582,6 +663,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,11 +980,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39077106-D844-481D-9CBA-D1EB2080F1CC}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G14:G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="D1" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="60"/>
+      <c r="G1" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="60"/>
+      <c r="J1" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="60"/>
+      <c r="M1" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" t="s">
+        <v>72</v>
+      </c>
+      <c r="M13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0752C00-C314-4AC1-BFCC-C3E780D9EA50}">
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +1230,7 @@
       </c>
       <c r="H1" s="31"/>
       <c r="I1" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J1" s="48"/>
       <c r="K1" s="30"/>
@@ -934,22 +1239,22 @@
         <v>2</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1" s="50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P1" s="32"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S1" s="42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T1" s="42"/>
       <c r="U1" s="42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="V1" s="43"/>
     </row>
@@ -966,16 +1271,16 @@
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>3</v>
@@ -983,7 +1288,7 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="8"/>
       <c r="U2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1000,14 +1305,14 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="O3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="8"/>
@@ -1025,7 +1330,7 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="7"/>
@@ -1041,7 +1346,7 @@
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
@@ -1051,14 +1356,14 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="8"/>
@@ -1085,7 +1390,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1093,7 +1398,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1157,9 +1462,9 @@
       <c r="J10" s="8"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="8"/>
     </row>
@@ -1176,9 +1481,9 @@
       <c r="J11" s="8"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="8"/>
     </row>
@@ -1190,16 +1495,18 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="11"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="M12" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="8"/>
     </row>
@@ -1216,9 +1523,9 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="8"/>
     </row>
@@ -1262,27 +1569,27 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="7"/>
       <c r="F16" s="2"/>
       <c r="G16" s="35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
       <c r="K16" s="7"/>
       <c r="L16" s="33"/>
       <c r="M16" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="20"/>
@@ -1292,30 +1599,30 @@
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="7"/>
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="7"/>
       <c r="L17" s="36"/>
       <c r="M17" s="21"/>
       <c r="N17" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O17" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="8"/>
@@ -1323,27 +1630,27 @@
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4"/>
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
       <c r="H18" s="51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" s="51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="7"/>
       <c r="L18" s="37"/>
       <c r="M18" s="27"/>
       <c r="N18" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O18" s="29"/>
       <c r="P18" s="7"/>
@@ -1352,7 +1659,7 @@
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8"/>
@@ -1360,17 +1667,17 @@
       <c r="F19" s="2"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="7"/>
       <c r="L19" s="39"/>
       <c r="M19" s="22"/>
       <c r="N19" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O19" s="24"/>
       <c r="P19" s="7"/>
@@ -1379,7 +1686,7 @@
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="40" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="8"/>
@@ -1387,7 +1694,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="6"/>
       <c r="H20" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="8"/>
@@ -1402,7 +1709,7 @@
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
@@ -1410,7 +1717,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="7"/>
       <c r="H21" s="40" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="I21" s="40"/>
       <c r="J21" s="8"/>
@@ -1425,7 +1732,7 @@
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
@@ -1433,17 +1740,17 @@
       <c r="F22" s="2"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
       <c r="K22" s="7"/>
       <c r="L22" s="33"/>
       <c r="M22" s="33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N22" s="33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O22" s="33"/>
       <c r="P22" s="7"/>
@@ -1458,7 +1765,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
@@ -1466,7 +1773,7 @@
       <c r="L23" s="33"/>
       <c r="M23" s="33"/>
       <c r="N23" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O23" s="33"/>
       <c r="P23" s="7"/>
@@ -1487,7 +1794,7 @@
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
       <c r="N24" s="33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O24" s="33"/>
       <c r="P24" s="7"/>
@@ -1508,7 +1815,7 @@
       <c r="L25" s="33"/>
       <c r="M25" s="33"/>
       <c r="N25" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O25" s="33"/>
       <c r="P25" s="7"/>
@@ -1529,7 +1836,7 @@
       <c r="L26" s="33"/>
       <c r="M26" s="33"/>
       <c r="N26" s="33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O26" s="33"/>
       <c r="P26" s="7"/>
@@ -1538,7 +1845,7 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="8"/>
@@ -1546,7 +1853,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
@@ -1573,7 +1880,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1581,7 +1888,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="2"/>
       <c r="G29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -1589,11 +1896,6 @@
       <c r="K29" s="7"/>
       <c r="L29" s="33"/>
       <c r="M29" s="33"/>
-      <c r="N29" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1610,9 +1912,6 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
       <c r="Q30" s="8"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1622,7 +1921,7 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -1642,25 +1941,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C059251-7E5B-47F6-9A8F-E7A0BC421FB2}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="55"/>
-    <col min="13" max="13" width="9.140625" style="55"/>
-    <col min="20" max="20" width="9.140625" style="55"/>
+    <col min="9" max="9" width="9.140625" style="55"/>
+    <col min="12" max="12" width="12" style="55" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>1</v>
       </c>
@@ -1670,69 +1970,70 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
       <c r="G1" s="57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="59" t="s">
+      <c r="I1" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="53"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="G2" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="55" t="s">
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="T2" s="55" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
       <c r="E3" s="60"/>
-      <c r="M3" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" s="55" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I3" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>